<commit_message>
Simplified partner tables and layout fixes
</commit_message>
<xml_diff>
--- a/docs/Chiraath-Business-Summary-Latest.xlsx
+++ b/docs/Chiraath-Business-Summary-Latest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anooppremachandran/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{777281BD-5DEB-BC45-8C82-B42B31633FF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{140994E9-0A30-D34D-BB08-95CF74168165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1742" uniqueCount="701">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1744" uniqueCount="702">
   <si>
     <t>Notes:</t>
   </si>
@@ -2188,6 +2188,9 @@
   </si>
   <si>
     <t>Saranya Gopalakrishnan(1250 pending)</t>
+  </si>
+  <si>
+    <t>Dec, Jan &amp; Feb boosting</t>
   </si>
 </sst>
 </file>
@@ -2546,7 +2549,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2793,9 +2796,6 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="25" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2950,7 +2950,7 @@
                   <c:v>47311</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1290</c:v>
+                  <c:v>4790</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -3323,7 +3323,7 @@
                   <c:v>-1863</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15899</c:v>
+                  <c:v>12399</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -7807,7 +7807,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B91" sqref="B91"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -7834,7 +7834,7 @@
       </c>
       <c r="B3" s="1">
         <f>SUM(Purchases!C:C)</f>
-        <v>253619</v>
+        <v>257119</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>39</v>
@@ -7883,7 +7883,7 @@
       </c>
       <c r="B6" s="52">
         <f>B4-B3</f>
-        <v>-30215</v>
+        <v>-33715</v>
       </c>
       <c r="E6" s="6" t="str">
         <f>PartnerShares!A5</f>
@@ -7918,7 +7918,7 @@
       </c>
       <c r="B10" s="52">
         <f>PartnerShares!H8</f>
-        <v>-429.66666666667152</v>
+        <v>-1596.3333333333285</v>
       </c>
       <c r="C10" s="6"/>
     </row>
@@ -7928,7 +7928,7 @@
       </c>
       <c r="B11" s="53">
         <f>PartnerShares!H9</f>
-        <v>-430.32666666667501</v>
+        <v>1903.006666666668</v>
       </c>
       <c r="C11" s="7"/>
     </row>
@@ -7938,7 +7938,7 @@
       </c>
       <c r="B12" s="52">
         <f>PartnerShares!H10</f>
-        <v>859.99333333333198</v>
+        <v>-306.67333333332499</v>
       </c>
       <c r="C12" s="6"/>
     </row>
@@ -7981,11 +7981,11 @@
       </c>
       <c r="C18" s="6">
         <f>PartnerShares!C8</f>
-        <v>84539.666666666672</v>
+        <v>85706.333333333328</v>
       </c>
       <c r="D18" s="6">
         <f>PartnerShares!D8</f>
-        <v>12884.333333333328</v>
+        <v>11717.666666666672</v>
       </c>
       <c r="E18" s="6">
         <f>IFERROR(SUMIFS(PartnerShares!$E$14:$E$500,PartnerShares!$D$14:$D$500,$A18,PartnerShares!$B$14:$B$500,"Contribution"),0)-IFERROR(SUMIFS(PartnerShares!$E$14:$E$500,PartnerShares!$C$14:$C$500,$A18,PartnerShares!$B$14:$B$500,"Contribution"),0)</f>
@@ -7993,7 +7993,7 @@
       </c>
       <c r="F18" s="8">
         <f>D18-E18</f>
-        <v>-429.66666666667152</v>
+        <v>-1596.3333333333285</v>
       </c>
       <c r="G18" s="71" t="s">
         <v>674</v>
@@ -8006,15 +8006,15 @@
       </c>
       <c r="B19" s="7">
         <f>PartnerShares!B9</f>
-        <v>130682</v>
+        <v>134182</v>
       </c>
       <c r="C19" s="7">
         <f>PartnerShares!C9</f>
-        <v>84539.666666666672</v>
+        <v>85706.333333333328</v>
       </c>
       <c r="D19" s="7">
         <f>PartnerShares!D9</f>
-        <v>46142.333333333328</v>
+        <v>48475.666666666672</v>
       </c>
       <c r="E19" s="7">
         <f>IFERROR(SUMIFS(PartnerShares!$E$14:$E$500,PartnerShares!$D$14:$D$500,$A19,PartnerShares!$B$14:$B$500,"Contribution"),0)-IFERROR(SUMIFS(PartnerShares!$E$14:$E$500,PartnerShares!$C$14:$C$500,$A19,PartnerShares!$B$14:$B$500,"Contribution"),0)</f>
@@ -8022,10 +8022,10 @@
       </c>
       <c r="F19" s="9">
         <f>D19-E19</f>
-        <v>-430.32666666667501</v>
-      </c>
-      <c r="G19" s="92" t="s">
-        <v>674</v>
+        <v>1903.006666666668</v>
+      </c>
+      <c r="G19" s="73" t="s">
+        <v>675</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -8039,11 +8039,11 @@
       </c>
       <c r="C20" s="6">
         <f>PartnerShares!C10</f>
-        <v>84539.666666666672</v>
+        <v>85706.333333333328</v>
       </c>
       <c r="D20" s="6">
         <f>PartnerShares!D10</f>
-        <v>-59026.666666666672</v>
+        <v>-60193.333333333328</v>
       </c>
       <c r="E20" s="6">
         <f>IFERROR(SUMIFS(PartnerShares!$E$14:$E$500,PartnerShares!$D$14:$D$500,$A20,PartnerShares!$B$14:$B$500,"Contribution"),0)-IFERROR(SUMIFS(PartnerShares!$E$14:$E$500,PartnerShares!$C$14:$C$500,$A20,PartnerShares!$B$14:$B$500,"Contribution"),0)</f>
@@ -8051,10 +8051,10 @@
       </c>
       <c r="F20" s="8">
         <f>D20-E20</f>
-        <v>859.99333333333198</v>
-      </c>
-      <c r="G20" s="73" t="s">
-        <v>675</v>
+        <v>-306.67333333332499</v>
+      </c>
+      <c r="G20" s="71" t="s">
+        <v>674</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="16" customHeight="1">
@@ -8254,16 +8254,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" customHeight="1">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="96" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="98"/>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="98"/>
-      <c r="H1" s="98"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="14" t="s">
@@ -8280,7 +8280,7 @@
       </c>
       <c r="B5" s="15">
         <f>Summary!B3</f>
-        <v>253619</v>
+        <v>257119</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>60</v>
@@ -8296,7 +8296,7 @@
       </c>
       <c r="B6" s="15">
         <f>Summary!B6</f>
-        <v>-30215</v>
+        <v>-33715</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>62</v>
@@ -8356,7 +8356,7 @@
       </c>
       <c r="B11" s="19">
         <f>IFERROR(SUMPRODUCT((TEXT(Purchases!$A$2:$A$998,"MMM")=$A11)*Purchases!$C$2:$C$998),0)</f>
-        <v>1290</v>
+        <v>4790</v>
       </c>
       <c r="C11" s="19">
         <f>IFERROR(SUMPRODUCT((TEXT(Sales!$A$2:$A$998,"MMM")=$A11)*Sales!$C$2:$C$998),0)</f>
@@ -8364,7 +8364,7 @@
       </c>
       <c r="D11" s="19">
         <f t="shared" si="0"/>
-        <v>15899</v>
+        <v>12399</v>
       </c>
       <c r="F11" s="18" t="s">
         <v>72</v>
@@ -8687,8 +8687,8 @@
   <dimension ref="A1:E450"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D48" sqref="A1:D48"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -8700,16 +8700,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="92" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="94" t="s">
+      <c r="B1" s="93" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="94" t="s">
+      <c r="C1" s="93" t="s">
         <v>84</v>
       </c>
-      <c r="D1" s="94" t="s">
+      <c r="D1" s="93" t="s">
         <v>85</v>
       </c>
     </row>
@@ -9373,10 +9373,18 @@
       <c r="E48" s="91"/>
     </row>
     <row r="49" spans="1:4">
-      <c r="A49" s="36"/>
-      <c r="B49" s="37"/>
-      <c r="C49" s="38"/>
-      <c r="D49" s="37"/>
+      <c r="A49" s="36">
+        <v>46078</v>
+      </c>
+      <c r="B49" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="C49" s="38">
+        <v>3500</v>
+      </c>
+      <c r="D49" s="37" t="s">
+        <v>701</v>
+      </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="41"/>
@@ -16378,65 +16386,65 @@
     <col min="21" max="16384" width="7" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="96" customFormat="1" ht="31" customHeight="1">
-      <c r="A1" s="95" t="s">
+    <row r="1" spans="1:20" s="95" customFormat="1" ht="31" customHeight="1">
+      <c r="A1" s="94" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="95" t="s">
+      <c r="B1" s="94" t="s">
         <v>103</v>
       </c>
-      <c r="C1" s="95" t="s">
+      <c r="C1" s="94" t="s">
         <v>104</v>
       </c>
-      <c r="D1" s="95" t="s">
+      <c r="D1" s="94" t="s">
         <v>105</v>
       </c>
-      <c r="E1" s="95" t="s">
+      <c r="E1" s="94" t="s">
         <v>106</v>
       </c>
-      <c r="F1" s="95" t="s">
+      <c r="F1" s="94" t="s">
         <v>70</v>
       </c>
-      <c r="G1" s="95" t="s">
+      <c r="G1" s="94" t="s">
         <v>72</v>
       </c>
-      <c r="H1" s="95" t="s">
+      <c r="H1" s="94" t="s">
         <v>107</v>
       </c>
-      <c r="I1" s="95" t="s">
+      <c r="I1" s="94" t="s">
         <v>108</v>
       </c>
-      <c r="J1" s="95" t="s">
+      <c r="J1" s="94" t="s">
         <v>109</v>
       </c>
-      <c r="K1" s="95" t="s">
+      <c r="K1" s="94" t="s">
         <v>110</v>
       </c>
-      <c r="L1" s="95" t="s">
+      <c r="L1" s="94" t="s">
         <v>111</v>
       </c>
-      <c r="M1" s="95" t="s">
+      <c r="M1" s="94" t="s">
         <v>112</v>
       </c>
-      <c r="N1" s="95" t="s">
+      <c r="N1" s="94" t="s">
         <v>52</v>
       </c>
-      <c r="O1" s="95" t="s">
+      <c r="O1" s="94" t="s">
         <v>113</v>
       </c>
-      <c r="P1" s="95" t="s">
+      <c r="P1" s="94" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="95" t="s">
+      <c r="Q1" s="94" t="s">
         <v>115</v>
       </c>
-      <c r="R1" s="95" t="s">
+      <c r="R1" s="94" t="s">
         <v>116</v>
       </c>
-      <c r="S1" s="95" t="s">
+      <c r="S1" s="94" t="s">
         <v>117</v>
       </c>
-      <c r="T1" s="95" t="s">
+      <c r="T1" s="94" t="s">
         <v>118</v>
       </c>
     </row>
@@ -25077,10 +25085,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="98" t="s">
         <v>291</v>
       </c>
-      <c r="B1" s="100"/>
+      <c r="B1" s="99"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
@@ -25150,11 +25158,11 @@
       </c>
       <c r="C8" s="6">
         <f>SUM($B$8:$B$10)/3</f>
-        <v>84539.666666666672</v>
+        <v>85706.333333333328</v>
       </c>
       <c r="D8" s="6">
         <f>B8-C8</f>
-        <v>12884.333333333328</v>
+        <v>11717.666666666672</v>
       </c>
       <c r="E8" s="6">
         <f>IF(Summary!$B$6&gt;0, Summary!$B$6*VLOOKUP($A8,$A$3:$B$5,2,FALSE),0)</f>
@@ -25162,7 +25170,7 @@
       </c>
       <c r="F8" s="6">
         <f>D8+E8</f>
-        <v>12884.333333333328</v>
+        <v>11717.666666666672</v>
       </c>
       <c r="G8" s="6">
         <f>IFERROR(SUMIFS($E$13:$E$499,$D$13:$D$499,$A8,$B$13:$B$499,"Contribution"),0)+IFERROR(SUMIFS($E$13:$E$499,$D$13:$D$499,$A8,$B$13:$B$499,"Profit"),0)-IFERROR(SUMIFS($E$13:$E$499,$C$13:$C$499,$A8,$B$13:$B$499,"Contribution"),0)-IFERROR(SUMIFS($E$13:$E$499,$C$13:$C$499,$A8,$B$13:$B$499,"Profit"),0)</f>
@@ -25170,7 +25178,7 @@
       </c>
       <c r="H8" s="8">
         <f>F8-G8</f>
-        <v>-429.66666666667152</v>
+        <v>-1596.3333333333285</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -25179,15 +25187,15 @@
       </c>
       <c r="B9" s="7">
         <f>IFERROR(SUMIF(Purchases!$B:$B,$A9,Purchases!$C:$C),0)</f>
-        <v>130682</v>
+        <v>134182</v>
       </c>
       <c r="C9" s="7">
         <f>SUM($B$8:$B$10)/3</f>
-        <v>84539.666666666672</v>
+        <v>85706.333333333328</v>
       </c>
       <c r="D9" s="7">
         <f>B9-C9</f>
-        <v>46142.333333333328</v>
+        <v>48475.666666666672</v>
       </c>
       <c r="E9" s="7">
         <f>IF(Summary!$B$6&gt;0, Summary!$B$6*VLOOKUP($A9,$A$3:$B$5,2,FALSE),0)</f>
@@ -25195,7 +25203,7 @@
       </c>
       <c r="F9" s="7">
         <f>D9+E9</f>
-        <v>46142.333333333328</v>
+        <v>48475.666666666672</v>
       </c>
       <c r="G9" s="7">
         <f>IFERROR(SUMIFS($E$13:$E$499,$D$13:$D$499,$A9,$B$13:$B$499,"Contribution"),0)+IFERROR(SUMIFS($E$13:$E$499,$D$13:$D$499,$A9,$B$13:$B$499,"Profit"),0)-IFERROR(SUMIFS($E$13:$E$499,$C$13:$C$499,$A9,$B$13:$B$499,"Contribution"),0)-IFERROR(SUMIFS($E$13:$E$499,$C$13:$C$499,$A9,$B$13:$B$499,"Profit"),0)</f>
@@ -25203,7 +25211,7 @@
       </c>
       <c r="H9" s="9">
         <f>F9-G9</f>
-        <v>-430.32666666667501</v>
+        <v>1903.006666666668</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -25216,11 +25224,11 @@
       </c>
       <c r="C10" s="6">
         <f>SUM($B$8:$B$10)/3</f>
-        <v>84539.666666666672</v>
+        <v>85706.333333333328</v>
       </c>
       <c r="D10" s="6">
         <f>B10-C10</f>
-        <v>-59026.666666666672</v>
+        <v>-60193.333333333328</v>
       </c>
       <c r="E10" s="6">
         <f>IF(Summary!$B$6&gt;0, Summary!$B$6*VLOOKUP($A10,$A$3:$B$5,2,FALSE),0)</f>
@@ -25228,7 +25236,7 @@
       </c>
       <c r="F10" s="6">
         <f>D10+E10</f>
-        <v>-59026.666666666672</v>
+        <v>-60193.333333333328</v>
       </c>
       <c r="G10" s="6">
         <f>IFERROR(SUMIFS($E$13:$E$499,$D$13:$D$499,$A10,$B$13:$B$499,"Contribution"),0)+IFERROR(SUMIFS($E$13:$E$499,$D$13:$D$499,$A10,$B$13:$B$499,"Profit"),0)-IFERROR(SUMIFS($E$13:$E$499,$C$13:$C$499,$A10,$B$13:$B$499,"Contribution"),0)-IFERROR(SUMIFS($E$13:$E$499,$C$13:$C$499,$A10,$B$13:$B$499,"Profit"),0)</f>
@@ -25236,18 +25244,18 @@
       </c>
       <c r="H10" s="8">
         <f>F10-G10</f>
-        <v>859.99333333333198</v>
+        <v>-306.67333333332499</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="22" customFormat="1" ht="16" customHeight="1">
-      <c r="A12" s="101" t="s">
+      <c r="A12" s="100" t="s">
         <v>300</v>
       </c>
-      <c r="B12" s="100"/>
-      <c r="C12" s="100"/>
-      <c r="D12" s="100"/>
-      <c r="E12" s="100"/>
-      <c r="F12" s="100"/>
+      <c r="B12" s="99"/>
+      <c r="C12" s="99"/>
+      <c r="D12" s="99"/>
+      <c r="E12" s="99"/>
+      <c r="F12" s="99"/>
     </row>
     <row r="13" spans="1:8" s="21" customFormat="1">
       <c r="A13" s="20" t="s">

</xml_diff>

<commit_message>
Laks & Rajitha payment updates
</commit_message>
<xml_diff>
--- a/docs/Chiraath-Business-Summary-Latest.xlsx
+++ b/docs/Chiraath-Business-Summary-Latest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anooppremachandran/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{140994E9-0A30-D34D-BB08-95CF74168165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{625CECDB-3A8B-6642-A100-7732FCE507DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1744" uniqueCount="702">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1755" uniqueCount="704">
   <si>
     <t>Notes:</t>
   </si>
@@ -1778,9 +1778,6 @@
   </si>
   <si>
     <t>2 Tusser embroidery(blue/green), Yellow tissue silk</t>
-  </si>
-  <si>
-    <t>Athulya (brick red)-789, Annie-600(Yellow)</t>
   </si>
   <si>
     <t>Anju, Annie(2-blue/green)</t>
@@ -2164,9 +2161,6 @@
   </si>
   <si>
     <t>Saranya Gopalakrishnan</t>
-  </si>
-  <si>
-    <t>Gpau</t>
   </si>
   <si>
     <t>Semi Silk Black and Cotton Silk Green</t>
@@ -2191,6 +2185,18 @@
   </si>
   <si>
     <t>Dec, Jan &amp; Feb boosting</t>
+  </si>
+  <si>
+    <t>Latha (500)</t>
+  </si>
+  <si>
+    <t>Rajitha</t>
+  </si>
+  <si>
+    <t>Athulya (brick red)-789, Annie-600(Yellow), Rajitha (Peach)-500</t>
+  </si>
+  <si>
+    <t>Tissue silk floral</t>
   </si>
 </sst>
 </file>
@@ -3068,7 +3074,7 @@
                   <c:v>45448</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17189</c:v>
+                  <c:v>18189</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -3323,7 +3329,7 @@
                   <c:v>-1863</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12399</c:v>
+                  <c:v>13399</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -3649,10 +3655,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>172</c:v>
+                  <c:v>174</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>113</c:v>
+                  <c:v>111</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3961,7 +3967,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>103</c:v>
+                  <c:v>105</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>67</c:v>
@@ -4084,7 +4090,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>55</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>53</c:v>
@@ -4517,7 +4523,7 @@
                   <c:v>58255</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44954.18</c:v>
+                  <c:v>44076.18</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1829</c:v>
@@ -7849,7 +7855,7 @@
       </c>
       <c r="B4" s="52">
         <f>SUMIFS(Sales!C:C, Sales!I:I, "Completed")</f>
-        <v>223404</v>
+        <v>225284</v>
       </c>
       <c r="E4" s="6" t="str">
         <f>PartnerShares!A3</f>
@@ -7866,7 +7872,7 @@
       </c>
       <c r="B5" s="53">
         <f>SUM(Sales!C:C)</f>
-        <v>228664</v>
+        <v>229664</v>
       </c>
       <c r="E5" s="7" t="str">
         <f>PartnerShares!A4</f>
@@ -7883,7 +7889,7 @@
       </c>
       <c r="B6" s="52">
         <f>B4-B3</f>
-        <v>-33715</v>
+        <v>-31835</v>
       </c>
       <c r="E6" s="6" t="str">
         <f>PartnerShares!A5</f>
@@ -7996,7 +8002,7 @@
         <v>-1596.3333333333285</v>
       </c>
       <c r="G18" s="71" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -8025,7 +8031,7 @@
         <v>1903.006666666668</v>
       </c>
       <c r="G19" s="73" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -8054,7 +8060,7 @@
         <v>-306.67333333332499</v>
       </c>
       <c r="G20" s="71" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="16" customHeight="1">
@@ -8092,15 +8098,15 @@
       </c>
       <c r="B26" s="6">
         <f>'Cash Pool'!B4</f>
-        <v>204255</v>
+        <v>206135</v>
       </c>
       <c r="C26" s="6">
         <f>'Cash Pool'!D4</f>
-        <v>74482.893599999996</v>
+        <v>75109.685599999997</v>
       </c>
       <c r="D26" s="6">
         <f>'Cash Pool'!E4</f>
-        <v>129772.1064</v>
+        <v>131025.3144</v>
       </c>
       <c r="E26" s="6">
         <f>'Cash Pool'!F4</f>
@@ -8108,10 +8114,10 @@
       </c>
       <c r="F26" s="8">
         <f>'Cash Pool'!G4</f>
-        <v>5718.6304000000091</v>
+        <v>6971.8384000000078</v>
       </c>
       <c r="G26" s="71" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -8125,11 +8131,11 @@
       </c>
       <c r="C27" s="7">
         <f>'Cash Pool'!D5</f>
-        <v>74438.212799999994</v>
+        <v>75064.628800000006</v>
       </c>
       <c r="D27" s="7">
         <f>'Cash Pool'!E5</f>
-        <v>-67819.212799999994</v>
+        <v>-68445.628800000006</v>
       </c>
       <c r="E27" s="7">
         <f>'Cash Pool'!F5</f>
@@ -8137,10 +8143,10 @@
       </c>
       <c r="F27" s="9">
         <f>'Cash Pool'!G5</f>
-        <v>-2858.2607999999891</v>
+        <v>-3484.6768000000011</v>
       </c>
       <c r="G27" s="72" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -8154,11 +8160,11 @@
       </c>
       <c r="C28" s="6">
         <f>'Cash Pool'!D6</f>
-        <v>74482.893599999996</v>
+        <v>75109.685599999997</v>
       </c>
       <c r="D28" s="6">
         <f>'Cash Pool'!E6</f>
-        <v>-61952.893599999996</v>
+        <v>-62579.685599999997</v>
       </c>
       <c r="E28" s="6">
         <f>'Cash Pool'!F6</f>
@@ -8166,10 +8172,10 @@
       </c>
       <c r="F28" s="8">
         <f>'Cash Pool'!G6</f>
-        <v>-2860.3695999999909</v>
+        <v>-3487.1615999999922</v>
       </c>
       <c r="G28" s="73" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="16" customHeight="1">
@@ -8271,7 +8277,7 @@
       </c>
       <c r="B3">
         <f ca="1">TODAY()</f>
-        <v>46077</v>
+        <v>46081</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -8287,7 +8293,7 @@
       </c>
       <c r="E5" s="15">
         <f>Summary!B4</f>
-        <v>223404</v>
+        <v>225284</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -8296,14 +8302,14 @@
       </c>
       <c r="B6" s="15">
         <f>Summary!B6</f>
-        <v>-33715</v>
+        <v>-31835</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>62</v>
       </c>
       <c r="E6" s="15">
         <f>SUMIFS(INVENTORY!K:K, INVENTORY!N:N, "&lt;&gt;Sold Out")</f>
-        <v>100189.68</v>
+        <v>99311.679999999993</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -8347,7 +8353,7 @@
       </c>
       <c r="G10" s="15">
         <f>SUM(INVENTORY!F:F)</f>
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -8360,18 +8366,18 @@
       </c>
       <c r="C11" s="19">
         <f>IFERROR(SUMPRODUCT((TEXT(Sales!$A$2:$A$998,"MMM")=$A11)*Sales!$C$2:$C$998),0)</f>
-        <v>17189</v>
+        <v>18189</v>
       </c>
       <c r="D11" s="19">
         <f t="shared" si="0"/>
-        <v>12399</v>
+        <v>13399</v>
       </c>
       <c r="F11" s="18" t="s">
         <v>72</v>
       </c>
       <c r="G11" s="19">
         <f>SUM(INVENTORY!G:G)</f>
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -8567,11 +8573,11 @@
       </c>
       <c r="G47" s="76">
         <f>SUMIF(INVENTORY!C:C, F47, INVENTORY!F:F)</f>
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H47" s="76">
         <f>SUMIF(INVENTORY!C:C, F47, INVENTORY!G:G)</f>
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J47" s="76" t="s">
         <v>135</v>
@@ -8598,7 +8604,7 @@
       </c>
       <c r="K48" s="77" cm="1">
         <f t="array" ref="K48">SUMPRODUCT((INVENTORY!$C$2:$C$479=J48)*(INVENTORY!$D$2:$D$479)*(INVENTORY!$G$2:$G$479))</f>
-        <v>44954.18</v>
+        <v>44076.18</v>
       </c>
     </row>
     <row r="49" spans="5:12">
@@ -9242,7 +9248,7 @@
         <v>5940</v>
       </c>
       <c r="D39" s="37" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -9284,7 +9290,7 @@
         <v>4425</v>
       </c>
       <c r="D42" s="39" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -9298,7 +9304,7 @@
         <v>1370</v>
       </c>
       <c r="D43" s="37" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -9326,7 +9332,7 @@
         <v>106</v>
       </c>
       <c r="D45" s="37" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -9368,7 +9374,7 @@
         <v>1290</v>
       </c>
       <c r="D48" s="39" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="E48" s="91"/>
     </row>
@@ -9383,7 +9389,7 @@
         <v>3500</v>
       </c>
       <c r="D49" s="37" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -11804,7 +11810,7 @@
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A100" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J124" sqref="J124"/>
+      <selection pane="bottomLeft" activeCell="J126" sqref="J126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -14031,7 +14037,7 @@
         <v>46035</v>
       </c>
       <c r="B93" s="47" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="C93" s="48">
         <v>1450</v>
@@ -14045,7 +14051,7 @@
       <c r="F93" s="49"/>
       <c r="G93" s="49"/>
       <c r="H93" s="68" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="I93" s="47" t="s">
         <v>276</v>
@@ -14056,7 +14062,7 @@
         <v>46036</v>
       </c>
       <c r="B94" s="50" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C94" s="51">
         <v>1599</v>
@@ -14070,7 +14076,7 @@
       <c r="F94" s="50"/>
       <c r="G94" s="50"/>
       <c r="H94" s="69" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="I94" s="50" t="s">
         <v>276</v>
@@ -14081,7 +14087,7 @@
         <v>46038</v>
       </c>
       <c r="B95" s="47" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C95" s="48">
         <v>1100</v>
@@ -14120,7 +14126,7 @@
       <c r="F96" s="50"/>
       <c r="G96" s="50"/>
       <c r="H96" s="69" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="I96" s="50" t="s">
         <v>276</v>
@@ -14131,7 +14137,7 @@
         <v>46039</v>
       </c>
       <c r="B97" s="47" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="C97" s="48">
         <v>2300</v>
@@ -14145,7 +14151,7 @@
       <c r="F97" s="49"/>
       <c r="G97" s="49"/>
       <c r="H97" s="68" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="I97" s="47" t="s">
         <v>276</v>
@@ -14156,7 +14162,7 @@
         <v>46040</v>
       </c>
       <c r="B98" s="50" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="C98" s="51">
         <v>1399</v>
@@ -14170,7 +14176,7 @@
       <c r="F98" s="50"/>
       <c r="G98" s="50"/>
       <c r="H98" s="69" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="I98" s="50" t="s">
         <v>276</v>
@@ -14181,7 +14187,7 @@
         <v>46041</v>
       </c>
       <c r="B99" s="47" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="C99" s="48">
         <v>1100</v>
@@ -14206,7 +14212,7 @@
         <v>46042</v>
       </c>
       <c r="B100" s="50" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="C100" s="51">
         <v>1250</v>
@@ -14220,7 +14226,7 @@
       <c r="F100" s="50"/>
       <c r="G100" s="50"/>
       <c r="H100" s="69" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="I100" s="50" t="s">
         <v>276</v>
@@ -14231,7 +14237,7 @@
         <v>46043</v>
       </c>
       <c r="B101" s="47" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C101" s="48">
         <v>1380</v>
@@ -14245,7 +14251,7 @@
       <c r="F101" s="49"/>
       <c r="G101" s="49"/>
       <c r="H101" s="68" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="I101" s="47" t="s">
         <v>276</v>
@@ -14256,7 +14262,7 @@
         <v>46046</v>
       </c>
       <c r="B102" s="50" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="C102" s="51">
         <v>950</v>
@@ -14270,7 +14276,7 @@
       <c r="F102" s="50"/>
       <c r="G102" s="50"/>
       <c r="H102" s="69" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="I102" s="50" t="s">
         <v>276</v>
@@ -14281,7 +14287,7 @@
         <v>46048</v>
       </c>
       <c r="B103" s="47" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="C103" s="48">
         <v>1380</v>
@@ -14306,7 +14312,7 @@
         <v>46048</v>
       </c>
       <c r="B104" s="50" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="C104" s="51">
         <v>2700</v>
@@ -14320,7 +14326,7 @@
       <c r="F104" s="50"/>
       <c r="G104" s="50"/>
       <c r="H104" s="69" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="I104" s="50" t="s">
         <v>276</v>
@@ -14331,7 +14337,7 @@
         <v>46049</v>
       </c>
       <c r="B105" s="47" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="C105" s="48">
         <v>1380</v>
@@ -14356,7 +14362,7 @@
         <v>46049</v>
       </c>
       <c r="B106" s="50" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="C106" s="51">
         <v>1380</v>
@@ -14370,7 +14376,7 @@
       <c r="F106" s="50"/>
       <c r="G106" s="50"/>
       <c r="H106" s="69" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="I106" s="50" t="s">
         <v>276</v>
@@ -14381,7 +14387,7 @@
         <v>46049</v>
       </c>
       <c r="B107" s="47" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="C107" s="48">
         <v>1200</v>
@@ -14395,7 +14401,7 @@
       <c r="F107" s="49"/>
       <c r="G107" s="49"/>
       <c r="H107" s="68" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="I107" s="47" t="s">
         <v>276</v>
@@ -14406,7 +14412,7 @@
         <v>46050</v>
       </c>
       <c r="B108" s="50" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="C108" s="51">
         <v>1250</v>
@@ -14420,7 +14426,7 @@
       <c r="F108" s="50"/>
       <c r="G108" s="50"/>
       <c r="H108" s="69" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="I108" s="50" t="s">
         <v>276</v>
@@ -14431,7 +14437,7 @@
         <v>46051</v>
       </c>
       <c r="B109" s="47" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="C109" s="48">
         <v>1380</v>
@@ -14456,7 +14462,7 @@
         <v>46051</v>
       </c>
       <c r="B110" s="50" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="C110" s="51">
         <v>1380</v>
@@ -14481,13 +14487,13 @@
         <v>46051</v>
       </c>
       <c r="B111" s="47" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="C111" s="48">
         <v>580</v>
       </c>
       <c r="D111" s="47" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E111" s="47" t="s">
         <v>48</v>
@@ -14495,7 +14501,7 @@
       <c r="F111" s="49"/>
       <c r="G111" s="49"/>
       <c r="H111" s="68" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="I111" s="47" t="s">
         <v>276</v>
@@ -14506,7 +14512,7 @@
         <v>46054</v>
       </c>
       <c r="B112" s="50" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="C112" s="51">
         <v>1800</v>
@@ -14520,7 +14526,7 @@
       <c r="F112" s="50"/>
       <c r="G112" s="50"/>
       <c r="H112" s="69" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="I112" s="50" t="s">
         <v>276</v>
@@ -14531,7 +14537,7 @@
         <v>46054</v>
       </c>
       <c r="B113" s="47" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="C113" s="48">
         <v>1550</v>
@@ -14545,7 +14551,7 @@
       <c r="F113" s="49"/>
       <c r="G113" s="49"/>
       <c r="H113" s="68" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="I113" s="47" t="s">
         <v>276</v>
@@ -14595,7 +14601,7 @@
       <c r="F115" s="49"/>
       <c r="G115" s="49"/>
       <c r="H115" s="68" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="I115" s="47" t="s">
         <v>191</v>
@@ -14606,7 +14612,7 @@
         <v>46060</v>
       </c>
       <c r="B116" s="50" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="C116" s="51">
         <v>1050</v>
@@ -14620,7 +14626,7 @@
       <c r="F116" s="50"/>
       <c r="G116" s="50"/>
       <c r="H116" s="69" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="I116" s="50" t="s">
         <v>276</v>
@@ -14631,7 +14637,7 @@
         <v>46062</v>
       </c>
       <c r="B117" s="47" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="C117" s="48">
         <v>1000</v>
@@ -14656,7 +14662,7 @@
         <v>46065</v>
       </c>
       <c r="B118" s="50" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="C118" s="51">
         <v>799</v>
@@ -14681,7 +14687,7 @@
         <v>46055</v>
       </c>
       <c r="B119" s="47" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="C119" s="48">
         <v>500</v>
@@ -14706,13 +14712,13 @@
         <v>46070</v>
       </c>
       <c r="B120" s="50" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="C120" s="51">
         <v>1450</v>
       </c>
       <c r="D120" s="50" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="E120" s="50" t="s">
         <v>46</v>
@@ -14720,7 +14726,7 @@
       <c r="F120" s="50"/>
       <c r="G120" s="50"/>
       <c r="H120" s="69" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="I120" s="50" t="s">
         <v>276</v>
@@ -14745,7 +14751,7 @@
       <c r="F121" s="49"/>
       <c r="G121" s="49"/>
       <c r="H121" s="68" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="I121" s="47" t="s">
         <v>276</v>
@@ -14756,7 +14762,7 @@
         <v>46074</v>
       </c>
       <c r="B122" s="50" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="C122" s="51">
         <v>1200</v>
@@ -14770,7 +14776,7 @@
       <c r="F122" s="50"/>
       <c r="G122" s="50"/>
       <c r="H122" s="69" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="I122" s="50" t="s">
         <v>276</v>
@@ -14781,7 +14787,7 @@
         <v>46075</v>
       </c>
       <c r="B123" s="47" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="C123" s="48">
         <v>1380</v>
@@ -14798,7 +14804,7 @@
         <v>491</v>
       </c>
       <c r="I123" s="47" t="s">
-        <v>191</v>
+        <v>276</v>
       </c>
     </row>
     <row r="124" spans="1:9">
@@ -14806,13 +14812,13 @@
         <v>46075</v>
       </c>
       <c r="B124" s="50" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="C124" s="51">
         <v>2500</v>
       </c>
       <c r="D124" s="50" t="s">
-        <v>695</v>
+        <v>281</v>
       </c>
       <c r="E124" s="50" t="s">
         <v>46</v>
@@ -14820,33 +14826,61 @@
       <c r="F124" s="50"/>
       <c r="G124" s="50"/>
       <c r="H124" s="69" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="I124" s="50" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="125" spans="1:9">
-      <c r="A125" s="46"/>
-      <c r="B125" s="47"/>
-      <c r="C125" s="48"/>
-      <c r="D125" s="47"/>
-      <c r="E125" s="47"/>
+    <row r="125" spans="1:9" ht="16">
+      <c r="A125" s="46">
+        <v>46079</v>
+      </c>
+      <c r="B125" s="47" t="s">
+        <v>128</v>
+      </c>
+      <c r="C125" s="48">
+        <v>500</v>
+      </c>
+      <c r="D125" s="47" t="s">
+        <v>281</v>
+      </c>
+      <c r="E125" s="47" t="s">
+        <v>46</v>
+      </c>
       <c r="F125" s="49"/>
       <c r="G125" s="49"/>
-      <c r="H125" s="68"/>
-      <c r="I125" s="47"/>
+      <c r="H125" s="68" t="s">
+        <v>245</v>
+      </c>
+      <c r="I125" s="47" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="126" spans="1:9">
-      <c r="A126" s="43"/>
-      <c r="B126" s="50"/>
-      <c r="C126" s="51"/>
-      <c r="D126" s="50"/>
-      <c r="E126" s="50"/>
+      <c r="A126" s="43">
+        <v>46079</v>
+      </c>
+      <c r="B126" s="50" t="s">
+        <v>701</v>
+      </c>
+      <c r="C126" s="51">
+        <v>500</v>
+      </c>
+      <c r="D126" s="50" t="s">
+        <v>281</v>
+      </c>
+      <c r="E126" s="50" t="s">
+        <v>46</v>
+      </c>
       <c r="F126" s="50"/>
       <c r="G126" s="50"/>
-      <c r="H126" s="69"/>
-      <c r="I126" s="50"/>
+      <c r="H126" s="69" t="s">
+        <v>703</v>
+      </c>
+      <c r="I126" s="50" t="s">
+        <v>276</v>
+      </c>
     </row>
     <row r="127" spans="1:9">
       <c r="A127" s="46"/>
@@ -16358,8 +16392,8 @@
   <dimension ref="A1:T176"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A123" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B132" sqref="B132"/>
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A92" sqref="A92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7" defaultRowHeight="14"/>
@@ -18921,10 +18955,10 @@
         <v>1094</v>
       </c>
       <c r="L47" s="28" t="s">
+        <v>569</v>
+      </c>
+      <c r="M47" s="28" t="s">
         <v>570</v>
-      </c>
-      <c r="M47" s="28" t="s">
-        <v>571</v>
       </c>
       <c r="N47" s="28" t="s">
         <v>180</v>
@@ -19193,7 +19227,7 @@
         <v>3600</v>
       </c>
       <c r="L52" s="30" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="M52" s="30"/>
       <c r="N52" s="30" t="s">
@@ -19249,7 +19283,7 @@
         <v>1941</v>
       </c>
       <c r="L53" s="28" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="M53" s="28"/>
       <c r="N53" s="28" t="s">
@@ -19259,7 +19293,7 @@
         <v>195</v>
       </c>
       <c r="P53" s="28" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="Q53" s="28"/>
       <c r="R53" s="28"/>
@@ -19361,7 +19395,7 @@
         <v>995</v>
       </c>
       <c r="L55" s="28" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="M55" s="28" t="s">
         <v>46</v>
@@ -19633,7 +19667,7 @@
         <v>1080</v>
       </c>
       <c r="L60" s="30" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="M60" s="30" t="s">
         <v>46</v>
@@ -19695,7 +19729,7 @@
       </c>
       <c r="O61" s="28"/>
       <c r="P61" s="28" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="Q61" s="28" t="s">
         <v>480</v>
@@ -19743,7 +19777,7 @@
         <v>562</v>
       </c>
       <c r="L62" s="30" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="M62" s="30"/>
       <c r="N62" s="30" t="s">
@@ -19949,7 +19983,7 @@
         <v>1558</v>
       </c>
       <c r="L66" s="30" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="M66" s="30"/>
       <c r="N66" s="30" t="s">
@@ -20121,7 +20155,7 @@
         <v>412</v>
       </c>
       <c r="B70" s="30" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C70" s="30" t="s">
         <v>120</v>
@@ -20155,7 +20189,7 @@
         <v>0</v>
       </c>
       <c r="L70" s="30" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="M70" s="30"/>
       <c r="N70" s="30" t="s">
@@ -20920,7 +20954,7 @@
         <v>180</v>
       </c>
       <c r="O84" s="30" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="P84" s="30"/>
       <c r="Q84" s="30"/>
@@ -20967,7 +21001,7 @@
         <v>895</v>
       </c>
       <c r="L85" s="28" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="M85" s="28"/>
       <c r="N85" s="28" t="s">
@@ -21021,7 +21055,7 @@
         <v>2090</v>
       </c>
       <c r="L86" s="30" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="M86" s="30"/>
       <c r="N86" s="30" t="s">
@@ -21194,7 +21228,7 @@
     </row>
     <row r="90" spans="1:20" ht="15" customHeight="1">
       <c r="A90" s="26" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B90" s="30" t="s">
         <v>244</v>
@@ -21231,7 +21265,7 @@
         <v>0</v>
       </c>
       <c r="L90" s="30" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="M90" s="30"/>
       <c r="N90" s="30" t="s">
@@ -21261,10 +21295,10 @@
         <v>689</v>
       </c>
       <c r="F91" s="29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G91" s="29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H91" s="28">
         <f t="shared" si="6"/>
@@ -21276,13 +21310,15 @@
       </c>
       <c r="J91" s="28">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>389</v>
       </c>
       <c r="K91" s="28">
         <f t="shared" si="8"/>
-        <v>778</v>
-      </c>
-      <c r="L91" s="28"/>
+        <v>389</v>
+      </c>
+      <c r="L91" s="28" t="s">
+        <v>700</v>
+      </c>
       <c r="M91" s="28"/>
       <c r="N91" s="28" t="s">
         <v>222</v>
@@ -21311,10 +21347,10 @@
         <v>789</v>
       </c>
       <c r="F92" s="31">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G92" s="31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H92" s="30">
         <f t="shared" si="6"/>
@@ -21326,18 +21362,18 @@
       </c>
       <c r="J92" s="30">
         <f t="shared" si="7"/>
-        <v>978</v>
+        <v>1467</v>
       </c>
       <c r="K92" s="30">
         <f t="shared" si="8"/>
-        <v>489</v>
+        <v>0</v>
       </c>
       <c r="L92" s="30" t="s">
-        <v>569</v>
+        <v>702</v>
       </c>
       <c r="M92" s="30"/>
       <c r="N92" s="30" t="s">
-        <v>180</v>
+        <v>122</v>
       </c>
       <c r="O92" s="30"/>
       <c r="P92" s="30"/>
@@ -22559,7 +22595,7 @@
         <v>3764.2799999999997</v>
       </c>
       <c r="L115" s="28" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="M115" s="28"/>
       <c r="N115" s="28" t="s">
@@ -22567,7 +22603,7 @@
       </c>
       <c r="O115" s="28"/>
       <c r="P115" s="89" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="Q115" s="28"/>
       <c r="R115" s="28"/>
@@ -22613,7 +22649,7 @@
         <v>891.5</v>
       </c>
       <c r="L116" s="30" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="M116" s="30"/>
       <c r="N116" s="30" t="s">
@@ -22621,7 +22657,7 @@
       </c>
       <c r="O116" s="30"/>
       <c r="P116" s="30" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="Q116" s="30"/>
       <c r="R116" s="30"/>
@@ -22989,7 +23025,7 @@
         <v>0</v>
       </c>
       <c r="L123" s="81" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="M123" s="81"/>
       <c r="N123" s="81" t="s">
@@ -23041,7 +23077,7 @@
         <v>0</v>
       </c>
       <c r="L124" s="84" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="M124" s="84"/>
       <c r="N124" s="84" t="s">
@@ -23095,7 +23131,7 @@
         <v>1816.5</v>
       </c>
       <c r="L125" s="81" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="M125" s="81"/>
       <c r="N125" s="81" t="s">
@@ -23221,7 +23257,7 @@
         <v>469</v>
       </c>
       <c r="B128" s="30" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C128" s="30" t="s">
         <v>120</v>
@@ -23271,7 +23307,7 @@
         <v>470</v>
       </c>
       <c r="B129" s="28" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C129" s="28" t="s">
         <v>120</v>
@@ -23321,7 +23357,7 @@
         <v>471</v>
       </c>
       <c r="B130" s="30" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C130" s="30" t="s">
         <v>120</v>
@@ -23371,7 +23407,7 @@
         <v>472</v>
       </c>
       <c r="B131" s="28" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="C131" s="28" t="s">
         <v>120</v>
@@ -23421,7 +23457,7 @@
         <v>473</v>
       </c>
       <c r="B132" s="30" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C132" s="30" t="s">
         <v>120</v>
@@ -23455,7 +23491,7 @@
         <v>0</v>
       </c>
       <c r="L132" s="30" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="M132" s="30"/>
       <c r="N132" s="30" t="s">
@@ -23473,7 +23509,7 @@
         <v>474</v>
       </c>
       <c r="B133" s="28" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="C133" s="28" t="s">
         <v>120</v>
@@ -23523,7 +23559,7 @@
         <v>475</v>
       </c>
       <c r="B134" s="30" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="C134" s="30" t="s">
         <v>120</v>
@@ -23573,7 +23609,7 @@
         <v>476</v>
       </c>
       <c r="B135" s="28" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="C135" s="28" t="s">
         <v>120</v>
@@ -23620,10 +23656,10 @@
     </row>
     <row r="136" spans="1:20" ht="15">
       <c r="A136" s="83" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B136" s="30" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="C136" s="30" t="s">
         <v>120</v>
@@ -23657,7 +23693,7 @@
         <v>1816</v>
       </c>
       <c r="L136" s="30" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="M136" s="30"/>
       <c r="N136" s="30" t="s">
@@ -23665,7 +23701,7 @@
       </c>
       <c r="O136" s="30"/>
       <c r="P136" s="30" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="Q136" s="30"/>
       <c r="R136" s="30"/>
@@ -23674,10 +23710,10 @@
     </row>
     <row r="137" spans="1:20" ht="15">
       <c r="A137" s="80" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B137" s="28" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C137" s="28" t="s">
         <v>120</v>
@@ -23726,10 +23762,10 @@
     </row>
     <row r="138" spans="1:20" ht="15">
       <c r="A138" s="83" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B138" s="30" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="C138" s="30" t="s">
         <v>120</v>
@@ -23776,10 +23812,10 @@
     </row>
     <row r="139" spans="1:20" ht="15">
       <c r="A139" s="80" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B139" s="28" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C139" s="28" t="s">
         <v>120</v>
@@ -23813,7 +23849,7 @@
         <v>0</v>
       </c>
       <c r="L139" s="28" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="M139" s="28"/>
       <c r="N139" s="28" t="s">
@@ -23828,10 +23864,10 @@
     </row>
     <row r="140" spans="1:20" ht="15">
       <c r="A140" s="83" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B140" s="30" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C140" s="30" t="s">
         <v>120</v>
@@ -23878,10 +23914,10 @@
     </row>
     <row r="141" spans="1:20" ht="15">
       <c r="A141" s="80" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B141" s="28" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C141" s="28" t="s">
         <v>120</v>
@@ -23928,10 +23964,10 @@
     </row>
     <row r="142" spans="1:20" ht="30">
       <c r="A142" s="30" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B142" s="30" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="C142" s="30" t="s">
         <v>120</v>
@@ -23965,7 +24001,7 @@
         <v>600</v>
       </c>
       <c r="L142" s="30" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="M142" s="30"/>
       <c r="N142" s="30" t="s">
@@ -23982,10 +24018,10 @@
     </row>
     <row r="143" spans="1:20" ht="15">
       <c r="A143" s="28" t="s">
+        <v>601</v>
+      </c>
+      <c r="B143" s="28" t="s">
         <v>602</v>
-      </c>
-      <c r="B143" s="28" t="s">
-        <v>603</v>
       </c>
       <c r="C143" s="28" t="s">
         <v>120</v>
@@ -24032,10 +24068,10 @@
     </row>
     <row r="144" spans="1:20" ht="15">
       <c r="A144" s="30" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B144" s="30" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="C144" s="30" t="s">
         <v>120</v>
@@ -24082,10 +24118,10 @@
     </row>
     <row r="145" spans="1:20" ht="15">
       <c r="A145" s="28" t="s">
+        <v>604</v>
+      </c>
+      <c r="B145" s="28" t="s">
         <v>605</v>
-      </c>
-      <c r="B145" s="28" t="s">
-        <v>606</v>
       </c>
       <c r="C145" s="28" t="s">
         <v>120</v>
@@ -24119,7 +24155,7 @@
         <v>0</v>
       </c>
       <c r="L145" s="28" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="M145" s="28"/>
       <c r="N145" s="28" t="s">
@@ -24134,10 +24170,10 @@
     </row>
     <row r="146" spans="1:20" ht="30">
       <c r="A146" s="30" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B146" s="30" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="C146" s="30" t="s">
         <v>120</v>
@@ -24184,10 +24220,10 @@
     </row>
     <row r="147" spans="1:20" ht="15">
       <c r="A147" s="28" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B147" s="28" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="C147" s="28" t="s">
         <v>120</v>
@@ -24234,10 +24270,10 @@
     </row>
     <row r="148" spans="1:20" ht="15">
       <c r="A148" s="30" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B148" s="30" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="C148" s="30" t="s">
         <v>120</v>
@@ -24284,10 +24320,10 @@
     </row>
     <row r="149" spans="1:20" ht="15">
       <c r="A149" s="28" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B149" s="28" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="C149" s="28" t="s">
         <v>120</v>
@@ -24334,10 +24370,10 @@
     </row>
     <row r="150" spans="1:20" ht="15">
       <c r="A150" s="30" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B150" s="30" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="C150" s="30" t="s">
         <v>120</v>
@@ -24384,10 +24420,10 @@
     </row>
     <row r="151" spans="1:20" ht="15">
       <c r="A151" s="28" t="s">
+        <v>624</v>
+      </c>
+      <c r="B151" s="28" t="s">
         <v>625</v>
-      </c>
-      <c r="B151" s="28" t="s">
-        <v>626</v>
       </c>
       <c r="C151" s="28" t="s">
         <v>135</v>
@@ -24426,10 +24462,10 @@
         <v>222</v>
       </c>
       <c r="O151" s="28" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="P151" s="28" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="Q151" s="28"/>
       <c r="R151" s="28"/>
@@ -24438,10 +24474,10 @@
     </row>
     <row r="152" spans="1:20" ht="15">
       <c r="A152" s="30" t="s">
+        <v>628</v>
+      </c>
+      <c r="B152" s="30" t="s">
         <v>629</v>
-      </c>
-      <c r="B152" s="30" t="s">
-        <v>630</v>
       </c>
       <c r="C152" s="30" t="s">
         <v>248</v>
@@ -24475,17 +24511,17 @@
         <v>885</v>
       </c>
       <c r="L152" s="30" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="M152" s="30"/>
       <c r="N152" s="30" t="s">
         <v>180</v>
       </c>
       <c r="O152" s="30" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="P152" s="30" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="Q152" s="30"/>
       <c r="R152" s="30"/>
@@ -24494,10 +24530,10 @@
     </row>
     <row r="153" spans="1:20" ht="15">
       <c r="A153" s="28" t="s">
+        <v>651</v>
+      </c>
+      <c r="B153" s="28" t="s">
         <v>652</v>
-      </c>
-      <c r="B153" s="28" t="s">
-        <v>653</v>
       </c>
       <c r="C153" s="28" t="s">
         <v>120</v>
@@ -24537,7 +24573,7 @@
       </c>
       <c r="O153" s="28"/>
       <c r="P153" s="28" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="Q153" s="28"/>
       <c r="R153" s="28"/>
@@ -25603,7 +25639,7 @@
       </c>
       <c r="B4" s="6">
         <f>IFERROR(SUMIFS(Sales!$C:$C,Sales!$E:$E,$A4,Sales!$I:$I,"Completed"),0)</f>
-        <v>204255</v>
+        <v>206135</v>
       </c>
       <c r="C4" s="6">
         <f>VLOOKUP($A4,PartnerShares!$A$3:$B$5,2,FALSE)</f>
@@ -25611,11 +25647,11 @@
       </c>
       <c r="D4" s="6">
         <f>Summary!$B$4*C4</f>
-        <v>74482.893599999996</v>
+        <v>75109.685599999997</v>
       </c>
       <c r="E4" s="6">
         <f>B4-D4</f>
-        <v>129772.1064</v>
+        <v>131025.3144</v>
       </c>
       <c r="F4" s="6">
         <f>IFERROR(SUMIFS(PartnerShares!$E$13:$E$499,PartnerShares!$D$13:$D$499,$A4,PartnerShares!$B$13:$B$499,"Cash"),0)-IFERROR(SUMIFS(PartnerShares!$E$13:$E$499,PartnerShares!$C$13:$C$499,$A4,PartnerShares!$B$13:$B$499,"Cash"),0)</f>
@@ -25623,7 +25659,7 @@
       </c>
       <c r="G4" s="8">
         <f>E4+F4</f>
-        <v>5718.6304000000091</v>
+        <v>6971.8384000000078</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -25640,11 +25676,11 @@
       </c>
       <c r="D5" s="7">
         <f>Summary!$B$4*C5</f>
-        <v>74438.212799999994</v>
+        <v>75064.628800000006</v>
       </c>
       <c r="E5" s="7">
         <f>B5-D5</f>
-        <v>-67819.212799999994</v>
+        <v>-68445.628800000006</v>
       </c>
       <c r="F5" s="7">
         <f>IFERROR(SUMIFS(PartnerShares!$E$13:$E$499,PartnerShares!$D$13:$D$499,$A5,PartnerShares!$B$13:$B$499,"Cash"),0)-IFERROR(SUMIFS(PartnerShares!$E$13:$E$499,PartnerShares!$C$13:$C$499,$A5,PartnerShares!$B$13:$B$499,"Cash"),0)</f>
@@ -25652,7 +25688,7 @@
       </c>
       <c r="G5" s="9">
         <f>E5+F5</f>
-        <v>-2858.2607999999891</v>
+        <v>-3484.6768000000011</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -25669,11 +25705,11 @@
       </c>
       <c r="D6" s="6">
         <f>Summary!$B$4*C6</f>
-        <v>74482.893599999996</v>
+        <v>75109.685599999997</v>
       </c>
       <c r="E6" s="6">
         <f>B6-D6</f>
-        <v>-61952.893599999996</v>
+        <v>-62579.685599999997</v>
       </c>
       <c r="F6" s="6">
         <f>IFERROR(SUMIFS(PartnerShares!$E$13:$E$499,PartnerShares!$D$13:$D$499,$A6,PartnerShares!$B$13:$B$499,"Cash"),0)-IFERROR(SUMIFS(PartnerShares!$E$13:$E$499,PartnerShares!$C$13:$C$499,$A6,PartnerShares!$B$13:$B$499,"Cash"),0)</f>
@@ -25681,7 +25717,7 @@
       </c>
       <c r="G6" s="8">
         <f>E6+F6</f>
-        <v>-2860.3695999999909</v>
+        <v>-3487.1615999999922</v>
       </c>
     </row>
     <row r="9" spans="1:7">

</xml_diff>